<commit_message>
Finish of create assessment
</commit_message>
<xml_diff>
--- a/frontend/web/uploads/PeerReviewTemplate.xlsx
+++ b/frontend/web/uploads/PeerReviewTemplate.xlsx
@@ -38,19 +38,19 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Marker Student Matriculation Number</t>
-  </si>
-  <si>
     <t>Work File</t>
   </si>
   <si>
-    <t>Marker Student First Name</t>
-  </si>
-  <si>
-    <t>Marker Student Last Name</t>
-  </si>
-  <si>
-    <t>Marker Student Email</t>
+    <t>Matriculation Number(Marker Student)</t>
+  </si>
+  <si>
+    <t>First Name(Marker Student)</t>
+  </si>
+  <si>
+    <t>Last Name(Marker Student)</t>
+  </si>
+  <si>
+    <t>Email(Marker Student)</t>
   </si>
 </sst>
 </file>
@@ -408,10 +408,10 @@
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -428,10 +428,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>

</xml_diff>